<commit_message>
Fix bugs, streaming video
</commit_message>
<xml_diff>
--- a/server/data/data.xlsx
+++ b/server/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vehicle-speed-estimation\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE5550F-27E1-4180-B060-073B8B3595BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED83DCBD-2301-434F-94E0-D284AC3A96AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4830" yWindow="2270" windowWidth="13700" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3803,7 +3803,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>